<commit_message>
session 4 and 5 written
</commit_message>
<xml_diff>
--- a/Data Science Bootcamp/syllabus.xlsx
+++ b/Data Science Bootcamp/syllabus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utpmy-my.sharepoint.com/personal/shahbalayev_18003701_utp_edu_my/Documents/Kurslar/UpData/Data Science Bootcamp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="364" documentId="8_{036567FC-2A41-46BE-81DB-C991EC6F65E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8ACD94B-42AD-4113-946D-8552DF3E28D4}"/>
+  <xr:revisionPtr revIDLastSave="365" documentId="8_{036567FC-2A41-46BE-81DB-C991EC6F65E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58DC32C0-2AE6-4C19-9671-CD44CAE0E1AC}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{25498CDB-D54D-4CAF-9778-4967BA85C4BF}"/>
+    <workbookView xWindow="22932" yWindow="-48" windowWidth="23256" windowHeight="12456" xr2:uid="{25498CDB-D54D-4CAF-9778-4967BA85C4BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1345,35 +1345,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1383,9 +1359,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1405,25 +1378,35 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1435,7 +1418,24 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1752,16 +1752,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D50690C7-F6D7-44A1-9252-D186C6665102}">
   <dimension ref="B1:T295"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28:D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.28515625" style="1"/>
-    <col min="2" max="2" width="27.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="82.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.42578125" style="1" customWidth="1"/>
     <col min="5" max="6" width="9.28515625" style="1"/>
     <col min="7" max="7" width="28.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
@@ -1773,2639 +1773,2655 @@
   <sheetData>
     <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="23"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="7" t="s">
+      <c r="B3" s="29"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="23"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="7" t="s">
+      <c r="B4" s="29"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="9" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="23"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="7" t="s">
+      <c r="B5" s="29"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="9" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="23"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="7" t="s">
+      <c r="B6" s="29"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="H6" s="9" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="23"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="7" t="s">
+      <c r="B7" s="29"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="4" t="s">
         <v>317</v>
       </c>
-      <c r="H7" s="18" t="s">
+      <c r="H7" s="9" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="23"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="7" t="s">
+      <c r="B8" s="29"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G8" s="4" t="s">
         <v>318</v>
       </c>
-      <c r="H8" s="18" t="s">
+      <c r="H8" s="9" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="23"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="7" t="s">
+      <c r="B9" s="29"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="H9" s="18" t="s">
+      <c r="H9" s="9" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="23"/>
-      <c r="C10" s="6" t="s">
+      <c r="B10" s="29"/>
+      <c r="C10" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="G10" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="H10" s="18" t="s">
+      <c r="H10" s="9" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="23"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="7" t="s">
+      <c r="B11" s="29"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="23"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="7" t="s">
+      <c r="B12" s="29"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="11" t="s">
+      <c r="G12" s="16" t="s">
         <v>324</v>
       </c>
-      <c r="H12" s="12" t="s">
+      <c r="H12" s="4" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="23"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="7" t="s">
+      <c r="B13" s="29"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="15"/>
-      <c r="H13" s="12" t="s">
+      <c r="G13" s="17"/>
+      <c r="H13" s="4" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="23"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="7" t="s">
+      <c r="B14" s="29"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="23"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="7" t="s">
+      <c r="B15" s="29"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="23"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="7" t="s">
+      <c r="B16" s="29"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="23"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="7" t="s">
+      <c r="B17" s="29"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="23"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="7" t="s">
+      <c r="B18" s="29"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="23"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="7" t="s">
+      <c r="B19" s="29"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="23"/>
-      <c r="C20" s="6" t="s">
+      <c r="B20" s="29"/>
+      <c r="C20" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="23"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="7" t="s">
+      <c r="B21" s="29"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="23"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="7" t="s">
+      <c r="B22" s="29"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="23"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="7" t="s">
+      <c r="B23" s="29"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="23"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="7" t="s">
+      <c r="B24" s="29"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="23"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="7" t="s">
+      <c r="B25" s="29"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="23"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="7" t="s">
+      <c r="B26" s="29"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="23"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="7" t="s">
+      <c r="B27" s="29"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="23"/>
-      <c r="C28" s="6" t="s">
+      <c r="B28" s="29"/>
+      <c r="C28" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="23"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="7" t="s">
+      <c r="B29" s="29"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="3" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="23"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="7" t="s">
+      <c r="B30" s="29"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="23"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="7" t="s">
+      <c r="B31" s="29"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="23"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="7" t="s">
+      <c r="B32" s="29"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="33" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B33" s="23"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="7" t="s">
+      <c r="B33" s="29"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="3" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="34" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B34" s="23"/>
-      <c r="C34" s="6" t="s">
+      <c r="B34" s="29"/>
+      <c r="C34" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D34" s="3" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="35" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B35" s="23"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="7" t="s">
+      <c r="B35" s="29"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="K35" s="32"/>
-      <c r="L35" s="32"/>
-      <c r="M35" s="32"/>
-      <c r="N35" s="32"/>
+      <c r="K35" s="15"/>
+      <c r="L35" s="15"/>
+      <c r="M35" s="15"/>
+      <c r="N35" s="15"/>
     </row>
     <row r="36" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B36" s="23"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="7" t="s">
+      <c r="B36" s="29"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="K36" s="32"/>
-      <c r="L36" s="32"/>
-      <c r="M36" s="32"/>
-      <c r="N36" s="32"/>
+      <c r="K36" s="15"/>
+      <c r="L36" s="15"/>
+      <c r="M36" s="15"/>
+      <c r="N36" s="15"/>
     </row>
     <row r="37" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B37" s="23"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="7" t="s">
+      <c r="B37" s="29"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="K37" s="32"/>
-      <c r="L37" s="32"/>
-      <c r="M37" s="32"/>
-      <c r="N37" s="32"/>
+      <c r="K37" s="15"/>
+      <c r="L37" s="15"/>
+      <c r="M37" s="15"/>
+      <c r="N37" s="15"/>
     </row>
     <row r="38" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B38" s="23"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="7" t="s">
+      <c r="B38" s="29"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="K38" s="32"/>
-      <c r="L38" s="32"/>
-      <c r="M38" s="32"/>
-      <c r="N38" s="32"/>
+      <c r="K38" s="15"/>
+      <c r="L38" s="15"/>
+      <c r="M38" s="15"/>
+      <c r="N38" s="15"/>
     </row>
     <row r="39" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B39" s="23"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="7" t="s">
+      <c r="B39" s="29"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="K39" s="32"/>
-      <c r="L39" s="32"/>
-      <c r="M39" s="32"/>
-      <c r="N39" s="32"/>
+      <c r="K39" s="15"/>
+      <c r="L39" s="15"/>
+      <c r="M39" s="15"/>
+      <c r="N39" s="15"/>
     </row>
     <row r="40" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B40" s="23"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="7" t="s">
+      <c r="B40" s="29"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="K40" s="32"/>
-      <c r="L40" s="32"/>
-      <c r="M40" s="32"/>
-      <c r="N40" s="32"/>
+      <c r="K40" s="15"/>
+      <c r="L40" s="15"/>
+      <c r="M40" s="15"/>
+      <c r="N40" s="15"/>
     </row>
     <row r="41" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B41" s="23"/>
-      <c r="C41" s="6" t="s">
+      <c r="B41" s="29"/>
+      <c r="C41" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D41" s="7" t="s">
+      <c r="D41" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="K41" s="32"/>
-      <c r="L41" s="32"/>
-      <c r="M41" s="32"/>
-      <c r="N41" s="32"/>
+      <c r="K41" s="15"/>
+      <c r="L41" s="15"/>
+      <c r="M41" s="15"/>
+      <c r="N41" s="15"/>
     </row>
     <row r="42" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B42" s="23"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="7" t="s">
+      <c r="B42" s="29"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="K42" s="32"/>
-      <c r="L42" s="32"/>
-      <c r="M42" s="32"/>
-      <c r="N42" s="32"/>
-      <c r="T42" s="14"/>
+      <c r="K42" s="15"/>
+      <c r="L42" s="15"/>
+      <c r="M42" s="15"/>
+      <c r="N42" s="15"/>
+      <c r="T42" s="6"/>
     </row>
     <row r="43" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B43" s="23"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="7" t="s">
+      <c r="B43" s="29"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="K43" s="32"/>
-      <c r="L43" s="32"/>
-      <c r="M43" s="32"/>
-      <c r="N43" s="32"/>
-      <c r="T43" s="14"/>
+      <c r="K43" s="15"/>
+      <c r="L43" s="15"/>
+      <c r="M43" s="15"/>
+      <c r="N43" s="15"/>
+      <c r="T43" s="6"/>
     </row>
     <row r="44" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B44" s="23"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="7" t="s">
+      <c r="B44" s="29"/>
+      <c r="C44" s="18"/>
+      <c r="D44" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="K44" s="32"/>
-      <c r="L44" s="32"/>
-      <c r="M44" s="32"/>
-      <c r="N44" s="32"/>
-      <c r="T44" s="14"/>
+      <c r="K44" s="15"/>
+      <c r="L44" s="15"/>
+      <c r="M44" s="15"/>
+      <c r="N44" s="15"/>
+      <c r="T44" s="6"/>
     </row>
     <row r="45" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B45" s="23"/>
-      <c r="C45" s="6"/>
-      <c r="D45" s="7" t="s">
+      <c r="B45" s="29"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="K45" s="32"/>
-      <c r="L45" s="32"/>
-      <c r="M45" s="32"/>
-      <c r="N45" s="32"/>
-      <c r="T45" s="14"/>
+      <c r="K45" s="15"/>
+      <c r="L45" s="15"/>
+      <c r="M45" s="15"/>
+      <c r="N45" s="15"/>
+      <c r="T45" s="6"/>
     </row>
     <row r="46" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="24"/>
-      <c r="C46" s="26" t="s">
+      <c r="B46" s="30"/>
+      <c r="C46" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="D46" s="27"/>
-      <c r="K46" s="32"/>
-      <c r="L46" s="32"/>
-      <c r="M46" s="32"/>
-      <c r="N46" s="32"/>
-      <c r="T46" s="14"/>
+      <c r="D46" s="32"/>
+      <c r="K46" s="15"/>
+      <c r="L46" s="15"/>
+      <c r="M46" s="15"/>
+      <c r="N46" s="15"/>
+      <c r="T46" s="6"/>
     </row>
     <row r="47" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="25" t="s">
+      <c r="B47" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="C47" s="28" t="s">
+      <c r="C47" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D47" s="16" t="s">
+      <c r="D47" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="K47" s="32"/>
-      <c r="L47" s="32"/>
-      <c r="M47" s="32"/>
-      <c r="N47" s="32"/>
-      <c r="T47" s="14"/>
+      <c r="K47" s="15"/>
+      <c r="L47" s="15"/>
+      <c r="M47" s="15"/>
+      <c r="N47" s="15"/>
+      <c r="T47" s="6"/>
     </row>
     <row r="48" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B48" s="22" t="s">
+      <c r="B48" s="28" t="s">
         <v>176</v>
       </c>
-      <c r="C48" s="21" t="s">
+      <c r="C48" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D48" s="4" t="s">
+      <c r="D48" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="K48" s="32"/>
-      <c r="L48" s="32"/>
-      <c r="M48" s="32"/>
-      <c r="N48" s="32"/>
-      <c r="T48" s="14"/>
+      <c r="K48" s="15"/>
+      <c r="L48" s="15"/>
+      <c r="M48" s="15"/>
+      <c r="N48" s="15"/>
+      <c r="T48" s="6"/>
     </row>
     <row r="49" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B49" s="23"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="7" t="s">
+      <c r="B49" s="29"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="K49" s="32"/>
-      <c r="L49" s="32"/>
-      <c r="M49" s="32"/>
-      <c r="N49" s="32"/>
-      <c r="T49" s="14"/>
+      <c r="K49" s="15"/>
+      <c r="L49" s="15"/>
+      <c r="M49" s="15"/>
+      <c r="N49" s="15"/>
+      <c r="T49" s="6"/>
     </row>
     <row r="50" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B50" s="23"/>
-      <c r="C50" s="18"/>
-      <c r="D50" s="7" t="s">
+      <c r="B50" s="29"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="K50" s="32"/>
-      <c r="L50" s="32"/>
-      <c r="M50" s="32"/>
-      <c r="N50" s="32"/>
-      <c r="T50" s="14"/>
+      <c r="K50" s="15"/>
+      <c r="L50" s="15"/>
+      <c r="M50" s="15"/>
+      <c r="N50" s="15"/>
+      <c r="T50" s="6"/>
     </row>
     <row r="51" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B51" s="23"/>
-      <c r="C51" s="18"/>
-      <c r="D51" s="7" t="s">
+      <c r="B51" s="29"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="K51" s="32"/>
-      <c r="L51" s="32"/>
-      <c r="M51" s="32"/>
-      <c r="N51" s="32"/>
-      <c r="T51" s="14"/>
+      <c r="K51" s="15"/>
+      <c r="L51" s="15"/>
+      <c r="M51" s="15"/>
+      <c r="N51" s="15"/>
+      <c r="T51" s="6"/>
     </row>
     <row r="52" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B52" s="23"/>
-      <c r="C52" s="18"/>
-      <c r="D52" s="7" t="s">
+      <c r="B52" s="29"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="K52" s="32"/>
-      <c r="L52" s="32"/>
-      <c r="M52" s="32"/>
-      <c r="N52" s="32"/>
-      <c r="T52" s="14"/>
+      <c r="K52" s="15"/>
+      <c r="L52" s="15"/>
+      <c r="M52" s="15"/>
+      <c r="N52" s="15"/>
+      <c r="T52" s="6"/>
     </row>
     <row r="53" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B53" s="23"/>
-      <c r="C53" s="18"/>
-      <c r="D53" s="7" t="s">
+      <c r="B53" s="29"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="K53" s="32"/>
-      <c r="L53" s="32"/>
-      <c r="M53" s="32"/>
-      <c r="N53" s="32"/>
-      <c r="T53" s="14"/>
+      <c r="K53" s="15"/>
+      <c r="L53" s="15"/>
+      <c r="M53" s="15"/>
+      <c r="N53" s="15"/>
+      <c r="T53" s="6"/>
     </row>
     <row r="54" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B54" s="23"/>
-      <c r="C54" s="18"/>
-      <c r="D54" s="7" t="s">
+      <c r="B54" s="29"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="K54" s="32"/>
-      <c r="L54" s="32"/>
-      <c r="M54" s="32"/>
-      <c r="N54" s="32"/>
-      <c r="T54" s="14"/>
+      <c r="K54" s="15"/>
+      <c r="L54" s="15"/>
+      <c r="M54" s="15"/>
+      <c r="N54" s="15"/>
+      <c r="T54" s="6"/>
     </row>
     <row r="55" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B55" s="23"/>
-      <c r="C55" s="18"/>
-      <c r="D55" s="7" t="s">
+      <c r="B55" s="29"/>
+      <c r="C55" s="9"/>
+      <c r="D55" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="K55" s="32"/>
-      <c r="L55" s="32"/>
-      <c r="M55" s="32"/>
-      <c r="N55" s="32"/>
-      <c r="T55" s="14"/>
+      <c r="K55" s="15"/>
+      <c r="L55" s="15"/>
+      <c r="M55" s="15"/>
+      <c r="N55" s="15"/>
+      <c r="T55" s="6"/>
     </row>
     <row r="56" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B56" s="23"/>
-      <c r="C56" s="18" t="s">
+      <c r="B56" s="29"/>
+      <c r="C56" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D56" s="7" t="s">
+      <c r="D56" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="K56" s="32"/>
-      <c r="L56" s="32"/>
-      <c r="M56" s="32"/>
-      <c r="N56" s="32"/>
-      <c r="T56" s="14"/>
+      <c r="K56" s="15"/>
+      <c r="L56" s="15"/>
+      <c r="M56" s="15"/>
+      <c r="N56" s="15"/>
+      <c r="T56" s="6"/>
     </row>
     <row r="57" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B57" s="23"/>
-      <c r="C57" s="18"/>
-      <c r="D57" s="7" t="s">
+      <c r="B57" s="29"/>
+      <c r="C57" s="9"/>
+      <c r="D57" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="K57" s="32"/>
-      <c r="L57" s="32"/>
-      <c r="M57" s="32"/>
-      <c r="N57" s="32"/>
-      <c r="T57" s="14"/>
+      <c r="K57" s="15"/>
+      <c r="L57" s="15"/>
+      <c r="M57" s="15"/>
+      <c r="N57" s="15"/>
+      <c r="T57" s="6"/>
     </row>
     <row r="58" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B58" s="23"/>
-      <c r="C58" s="18"/>
-      <c r="D58" s="7" t="s">
+      <c r="B58" s="29"/>
+      <c r="C58" s="9"/>
+      <c r="D58" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="K58" s="32"/>
-      <c r="L58" s="32"/>
-      <c r="M58" s="32"/>
-      <c r="N58" s="32"/>
-      <c r="T58" s="14"/>
+      <c r="K58" s="15"/>
+      <c r="L58" s="15"/>
+      <c r="M58" s="15"/>
+      <c r="N58" s="15"/>
+      <c r="T58" s="6"/>
     </row>
     <row r="59" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B59" s="23"/>
-      <c r="C59" s="18"/>
-      <c r="D59" s="7" t="s">
+      <c r="B59" s="29"/>
+      <c r="C59" s="9"/>
+      <c r="D59" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="K59" s="32"/>
-      <c r="L59" s="32"/>
-      <c r="M59" s="32"/>
-      <c r="N59" s="32"/>
-      <c r="T59" s="14"/>
+      <c r="K59" s="15"/>
+      <c r="L59" s="15"/>
+      <c r="M59" s="15"/>
+      <c r="N59" s="15"/>
+      <c r="T59" s="6"/>
     </row>
     <row r="60" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B60" s="23"/>
-      <c r="C60" s="18"/>
-      <c r="D60" s="7" t="s">
+      <c r="B60" s="29"/>
+      <c r="C60" s="9"/>
+      <c r="D60" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="K60" s="32"/>
-      <c r="L60" s="32"/>
-      <c r="M60" s="32"/>
-      <c r="N60" s="32"/>
-      <c r="T60" s="14"/>
+      <c r="K60" s="15"/>
+      <c r="L60" s="15"/>
+      <c r="M60" s="15"/>
+      <c r="N60" s="15"/>
+      <c r="T60" s="6"/>
     </row>
     <row r="61" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B61" s="23"/>
-      <c r="C61" s="18" t="s">
+      <c r="B61" s="29"/>
+      <c r="C61" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D61" s="7" t="s">
+      <c r="D61" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="K61" s="32"/>
-      <c r="L61" s="32"/>
-      <c r="M61" s="32"/>
-      <c r="N61" s="32"/>
-      <c r="T61" s="14"/>
+      <c r="K61" s="15"/>
+      <c r="L61" s="15"/>
+      <c r="M61" s="15"/>
+      <c r="N61" s="15"/>
+      <c r="T61" s="6"/>
     </row>
     <row r="62" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B62" s="23"/>
-      <c r="C62" s="18"/>
-      <c r="D62" s="7" t="s">
+      <c r="B62" s="29"/>
+      <c r="C62" s="9"/>
+      <c r="D62" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="K62" s="32"/>
-      <c r="L62" s="32"/>
-      <c r="M62" s="32"/>
-      <c r="N62" s="32"/>
-      <c r="T62" s="14"/>
+      <c r="K62" s="15"/>
+      <c r="L62" s="15"/>
+      <c r="M62" s="15"/>
+      <c r="N62" s="15"/>
+      <c r="T62" s="6"/>
     </row>
     <row r="63" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B63" s="23"/>
-      <c r="C63" s="18"/>
-      <c r="D63" s="7" t="s">
+      <c r="B63" s="29"/>
+      <c r="C63" s="9"/>
+      <c r="D63" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="K63" s="32"/>
-      <c r="L63" s="32"/>
-      <c r="M63" s="32"/>
-      <c r="N63" s="32"/>
-      <c r="T63" s="14"/>
+      <c r="K63" s="15"/>
+      <c r="L63" s="15"/>
+      <c r="M63" s="15"/>
+      <c r="N63" s="15"/>
+      <c r="T63" s="6"/>
     </row>
     <row r="64" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B64" s="23"/>
-      <c r="C64" s="18"/>
-      <c r="D64" s="7" t="s">
+      <c r="B64" s="29"/>
+      <c r="C64" s="9"/>
+      <c r="D64" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="K64" s="32"/>
-      <c r="L64" s="32"/>
-      <c r="M64" s="32"/>
-      <c r="N64" s="32"/>
-      <c r="T64" s="14"/>
+      <c r="K64" s="15"/>
+      <c r="L64" s="15"/>
+      <c r="M64" s="15"/>
+      <c r="N64" s="15"/>
+      <c r="T64" s="6"/>
     </row>
     <row r="65" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B65" s="23"/>
-      <c r="C65" s="18"/>
-      <c r="D65" s="7" t="s">
+      <c r="B65" s="29"/>
+      <c r="C65" s="9"/>
+      <c r="D65" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="K65" s="32"/>
-      <c r="L65" s="32"/>
-      <c r="M65" s="32"/>
-      <c r="N65" s="32"/>
-      <c r="T65" s="14"/>
+      <c r="K65" s="15"/>
+      <c r="L65" s="15"/>
+      <c r="M65" s="15"/>
+      <c r="N65" s="15"/>
+      <c r="T65" s="6"/>
     </row>
     <row r="66" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B66" s="23"/>
-      <c r="C66" s="18"/>
-      <c r="D66" s="7" t="s">
+      <c r="B66" s="29"/>
+      <c r="C66" s="9"/>
+      <c r="D66" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="K66" s="32"/>
-      <c r="L66" s="32"/>
-      <c r="M66" s="32"/>
-      <c r="N66" s="32"/>
-      <c r="T66" s="14"/>
+      <c r="K66" s="15"/>
+      <c r="L66" s="15"/>
+      <c r="M66" s="15"/>
+      <c r="N66" s="15"/>
+      <c r="T66" s="6"/>
     </row>
     <row r="67" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B67" s="23"/>
-      <c r="C67" s="18"/>
-      <c r="D67" s="7" t="s">
+      <c r="B67" s="29"/>
+      <c r="C67" s="9"/>
+      <c r="D67" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="K67" s="32"/>
-      <c r="L67" s="32"/>
-      <c r="M67" s="32"/>
-      <c r="N67" s="32"/>
-      <c r="T67" s="14"/>
+      <c r="K67" s="15"/>
+      <c r="L67" s="15"/>
+      <c r="M67" s="15"/>
+      <c r="N67" s="15"/>
+      <c r="T67" s="6"/>
     </row>
     <row r="68" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B68" s="23"/>
-      <c r="C68" s="18" t="s">
+      <c r="B68" s="29"/>
+      <c r="C68" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D68" s="7" t="s">
+      <c r="D68" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="K68" s="32"/>
-      <c r="L68" s="32"/>
-      <c r="M68" s="32"/>
-      <c r="N68" s="32"/>
-      <c r="T68" s="14"/>
+      <c r="K68" s="15"/>
+      <c r="L68" s="15"/>
+      <c r="M68" s="15"/>
+      <c r="N68" s="15"/>
+      <c r="T68" s="6"/>
     </row>
     <row r="69" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B69" s="23"/>
-      <c r="C69" s="18"/>
-      <c r="D69" s="7" t="s">
+      <c r="B69" s="29"/>
+      <c r="C69" s="9"/>
+      <c r="D69" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="K69" s="32"/>
-      <c r="L69" s="32"/>
-      <c r="M69" s="32"/>
-      <c r="N69" s="32"/>
-      <c r="T69" s="14"/>
+      <c r="K69" s="15"/>
+      <c r="L69" s="15"/>
+      <c r="M69" s="15"/>
+      <c r="N69" s="15"/>
+      <c r="T69" s="6"/>
     </row>
     <row r="70" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B70" s="23"/>
-      <c r="C70" s="18"/>
-      <c r="D70" s="7" t="s">
+      <c r="B70" s="29"/>
+      <c r="C70" s="9"/>
+      <c r="D70" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="K70" s="32"/>
-      <c r="L70" s="32"/>
-      <c r="M70" s="32"/>
-      <c r="N70" s="32"/>
-      <c r="T70" s="14"/>
+      <c r="K70" s="15"/>
+      <c r="L70" s="15"/>
+      <c r="M70" s="15"/>
+      <c r="N70" s="15"/>
+      <c r="T70" s="6"/>
     </row>
     <row r="71" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B71" s="23"/>
-      <c r="C71" s="18"/>
-      <c r="D71" s="7" t="s">
+      <c r="B71" s="29"/>
+      <c r="C71" s="9"/>
+      <c r="D71" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="K71" s="32"/>
-      <c r="L71" s="32"/>
-      <c r="M71" s="32"/>
-      <c r="N71" s="32"/>
-      <c r="T71" s="14"/>
+      <c r="K71" s="15"/>
+      <c r="L71" s="15"/>
+      <c r="M71" s="15"/>
+      <c r="N71" s="15"/>
+      <c r="T71" s="6"/>
     </row>
     <row r="72" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B72" s="23"/>
-      <c r="C72" s="18" t="s">
+      <c r="B72" s="29"/>
+      <c r="C72" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D72" s="7" t="s">
+      <c r="D72" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="K72" s="32"/>
-      <c r="L72" s="32"/>
-      <c r="M72" s="32"/>
-      <c r="N72" s="32"/>
-      <c r="T72" s="14"/>
+      <c r="K72" s="15"/>
+      <c r="L72" s="15"/>
+      <c r="M72" s="15"/>
+      <c r="N72" s="15"/>
+      <c r="T72" s="6"/>
     </row>
     <row r="73" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B73" s="23"/>
-      <c r="C73" s="18"/>
-      <c r="D73" s="7" t="s">
+      <c r="B73" s="29"/>
+      <c r="C73" s="9"/>
+      <c r="D73" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="K73" s="32"/>
-      <c r="L73" s="32"/>
-      <c r="M73" s="32"/>
-      <c r="N73" s="32"/>
-      <c r="T73" s="14"/>
+      <c r="K73" s="15"/>
+      <c r="L73" s="15"/>
+      <c r="M73" s="15"/>
+      <c r="N73" s="15"/>
+      <c r="T73" s="6"/>
     </row>
     <row r="74" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B74" s="23"/>
-      <c r="C74" s="18"/>
-      <c r="D74" s="7" t="s">
+      <c r="B74" s="29"/>
+      <c r="C74" s="9"/>
+      <c r="D74" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="K74" s="32"/>
-      <c r="L74" s="32"/>
-      <c r="M74" s="32"/>
-      <c r="N74" s="32"/>
-      <c r="T74" s="14"/>
+      <c r="K74" s="15"/>
+      <c r="L74" s="15"/>
+      <c r="M74" s="15"/>
+      <c r="N74" s="15"/>
+      <c r="T74" s="6"/>
     </row>
     <row r="75" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B75" s="23"/>
-      <c r="C75" s="18"/>
-      <c r="D75" s="7" t="s">
+      <c r="B75" s="29"/>
+      <c r="C75" s="9"/>
+      <c r="D75" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="K75" s="32"/>
-      <c r="L75" s="32"/>
-      <c r="M75" s="32"/>
-      <c r="N75" s="32"/>
-      <c r="T75" s="14"/>
+      <c r="K75" s="15"/>
+      <c r="L75" s="15"/>
+      <c r="M75" s="15"/>
+      <c r="N75" s="15"/>
+      <c r="T75" s="6"/>
     </row>
     <row r="76" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B76" s="23"/>
-      <c r="C76" s="18"/>
-      <c r="D76" s="7" t="s">
+      <c r="B76" s="29"/>
+      <c r="C76" s="9"/>
+      <c r="D76" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="K76" s="32"/>
-      <c r="L76" s="32"/>
-      <c r="M76" s="32"/>
-      <c r="N76" s="32"/>
-      <c r="T76" s="14"/>
+      <c r="K76" s="15"/>
+      <c r="L76" s="15"/>
+      <c r="M76" s="15"/>
+      <c r="N76" s="15"/>
+      <c r="T76" s="6"/>
     </row>
     <row r="77" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B77" s="23"/>
-      <c r="C77" s="18" t="s">
+      <c r="B77" s="29"/>
+      <c r="C77" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D77" s="7" t="s">
+      <c r="D77" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="K77" s="32"/>
-      <c r="L77" s="32"/>
-      <c r="M77" s="32"/>
-      <c r="N77" s="32"/>
-      <c r="T77" s="14"/>
+      <c r="K77" s="15"/>
+      <c r="L77" s="15"/>
+      <c r="M77" s="15"/>
+      <c r="N77" s="15"/>
+      <c r="T77" s="6"/>
     </row>
     <row r="78" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B78" s="23"/>
-      <c r="C78" s="18"/>
-      <c r="D78" s="7" t="s">
+      <c r="B78" s="29"/>
+      <c r="C78" s="9"/>
+      <c r="D78" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="K78" s="32"/>
-      <c r="L78" s="32"/>
-      <c r="M78" s="32"/>
-      <c r="N78" s="32"/>
-      <c r="T78" s="14"/>
+      <c r="K78" s="15"/>
+      <c r="L78" s="15"/>
+      <c r="M78" s="15"/>
+      <c r="N78" s="15"/>
+      <c r="T78" s="6"/>
     </row>
     <row r="79" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B79" s="23"/>
-      <c r="C79" s="18"/>
-      <c r="D79" s="7" t="s">
+      <c r="B79" s="29"/>
+      <c r="C79" s="9"/>
+      <c r="D79" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="K79" s="32"/>
-      <c r="L79" s="32"/>
-      <c r="M79" s="32"/>
-      <c r="N79" s="32"/>
-      <c r="T79" s="14"/>
+      <c r="K79" s="15"/>
+      <c r="L79" s="15"/>
+      <c r="M79" s="15"/>
+      <c r="N79" s="15"/>
+      <c r="T79" s="6"/>
     </row>
     <row r="80" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B80" s="23"/>
-      <c r="C80" s="18"/>
-      <c r="D80" s="7" t="s">
+      <c r="B80" s="29"/>
+      <c r="C80" s="9"/>
+      <c r="D80" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="K80" s="32"/>
-      <c r="L80" s="32"/>
-      <c r="M80" s="32"/>
-      <c r="N80" s="32"/>
-      <c r="T80" s="14"/>
+      <c r="K80" s="15"/>
+      <c r="L80" s="15"/>
+      <c r="M80" s="15"/>
+      <c r="N80" s="15"/>
+      <c r="T80" s="6"/>
     </row>
     <row r="81" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B81" s="23"/>
-      <c r="C81" s="18"/>
-      <c r="D81" s="7" t="s">
+      <c r="B81" s="29"/>
+      <c r="C81" s="9"/>
+      <c r="D81" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="K81" s="32"/>
-      <c r="L81" s="32"/>
-      <c r="M81" s="32"/>
-      <c r="N81" s="32"/>
-      <c r="T81" s="14"/>
+      <c r="K81" s="15"/>
+      <c r="L81" s="15"/>
+      <c r="M81" s="15"/>
+      <c r="N81" s="15"/>
+      <c r="T81" s="6"/>
     </row>
     <row r="82" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B82" s="23"/>
-      <c r="C82" s="18"/>
-      <c r="D82" s="7" t="s">
+      <c r="B82" s="29"/>
+      <c r="C82" s="9"/>
+      <c r="D82" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="K82" s="32"/>
-      <c r="L82" s="32"/>
-      <c r="M82" s="32"/>
-      <c r="N82" s="32"/>
-      <c r="T82" s="14"/>
+      <c r="K82" s="15"/>
+      <c r="L82" s="15"/>
+      <c r="M82" s="15"/>
+      <c r="N82" s="15"/>
+      <c r="T82" s="6"/>
     </row>
     <row r="83" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B83" s="23"/>
-      <c r="C83" s="18" t="s">
+      <c r="B83" s="29"/>
+      <c r="C83" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="D83" s="7" t="s">
+      <c r="D83" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="K83" s="32"/>
-      <c r="L83" s="32"/>
-      <c r="M83" s="32"/>
-      <c r="N83" s="32"/>
-      <c r="T83" s="14"/>
+      <c r="K83" s="15"/>
+      <c r="L83" s="15"/>
+      <c r="M83" s="15"/>
+      <c r="N83" s="15"/>
+      <c r="T83" s="6"/>
     </row>
     <row r="84" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B84" s="23"/>
-      <c r="C84" s="18"/>
-      <c r="D84" s="7" t="s">
+      <c r="B84" s="29"/>
+      <c r="C84" s="9"/>
+      <c r="D84" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="K84" s="32"/>
-      <c r="L84" s="32"/>
-      <c r="M84" s="32"/>
-      <c r="N84" s="32"/>
-      <c r="T84" s="14"/>
+      <c r="K84" s="15"/>
+      <c r="L84" s="15"/>
+      <c r="M84" s="15"/>
+      <c r="N84" s="15"/>
+      <c r="T84" s="6"/>
     </row>
     <row r="85" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B85" s="23"/>
-      <c r="C85" s="18"/>
-      <c r="D85" s="7" t="s">
+      <c r="B85" s="29"/>
+      <c r="C85" s="9"/>
+      <c r="D85" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="K85" s="32"/>
-      <c r="L85" s="32"/>
-      <c r="M85" s="32"/>
-      <c r="N85" s="32"/>
-      <c r="T85" s="14"/>
+      <c r="K85" s="15"/>
+      <c r="L85" s="15"/>
+      <c r="M85" s="15"/>
+      <c r="N85" s="15"/>
+      <c r="T85" s="6"/>
     </row>
     <row r="86" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B86" s="23"/>
-      <c r="C86" s="18"/>
-      <c r="D86" s="7" t="s">
+      <c r="B86" s="29"/>
+      <c r="C86" s="9"/>
+      <c r="D86" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="K86" s="32"/>
-      <c r="L86" s="32"/>
-      <c r="M86" s="32"/>
-      <c r="N86" s="32"/>
-      <c r="T86" s="14"/>
+      <c r="K86" s="15"/>
+      <c r="L86" s="15"/>
+      <c r="M86" s="15"/>
+      <c r="N86" s="15"/>
+      <c r="T86" s="6"/>
     </row>
     <row r="87" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B87" s="23"/>
-      <c r="C87" s="18"/>
-      <c r="D87" s="7" t="s">
+      <c r="B87" s="29"/>
+      <c r="C87" s="9"/>
+      <c r="D87" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="K87" s="32"/>
-      <c r="L87" s="32"/>
-      <c r="M87" s="32"/>
-      <c r="N87" s="32"/>
-      <c r="T87" s="14"/>
+      <c r="K87" s="15"/>
+      <c r="L87" s="15"/>
+      <c r="M87" s="15"/>
+      <c r="N87" s="15"/>
+      <c r="T87" s="6"/>
     </row>
     <row r="88" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B88" s="23"/>
-      <c r="C88" s="18"/>
-      <c r="D88" s="7" t="s">
+      <c r="B88" s="29"/>
+      <c r="C88" s="9"/>
+      <c r="D88" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="K88" s="32"/>
-      <c r="L88" s="32"/>
-      <c r="M88" s="32"/>
-      <c r="N88" s="32"/>
-      <c r="T88" s="14"/>
+      <c r="K88" s="15"/>
+      <c r="L88" s="15"/>
+      <c r="M88" s="15"/>
+      <c r="N88" s="15"/>
+      <c r="T88" s="6"/>
     </row>
     <row r="89" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B89" s="23"/>
-      <c r="C89" s="18" t="s">
+      <c r="B89" s="29"/>
+      <c r="C89" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="D89" s="7" t="s">
+      <c r="D89" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="K89" s="32"/>
-      <c r="L89" s="32"/>
-      <c r="M89" s="32"/>
-      <c r="N89" s="32"/>
-      <c r="T89" s="14"/>
+      <c r="K89" s="15"/>
+      <c r="L89" s="15"/>
+      <c r="M89" s="15"/>
+      <c r="N89" s="15"/>
+      <c r="T89" s="6"/>
     </row>
     <row r="90" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B90" s="23"/>
-      <c r="C90" s="18"/>
-      <c r="D90" s="7" t="s">
+      <c r="B90" s="29"/>
+      <c r="C90" s="9"/>
+      <c r="D90" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="K90" s="32"/>
-      <c r="L90" s="32"/>
-      <c r="M90" s="32"/>
-      <c r="N90" s="32"/>
-      <c r="T90" s="14"/>
+      <c r="K90" s="15"/>
+      <c r="L90" s="15"/>
+      <c r="M90" s="15"/>
+      <c r="N90" s="15"/>
+      <c r="T90" s="6"/>
     </row>
     <row r="91" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B91" s="23"/>
-      <c r="C91" s="18"/>
-      <c r="D91" s="7" t="s">
+      <c r="B91" s="29"/>
+      <c r="C91" s="9"/>
+      <c r="D91" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="K91" s="32"/>
-      <c r="L91" s="32"/>
-      <c r="M91" s="32"/>
-      <c r="N91" s="32"/>
-      <c r="T91" s="14"/>
+      <c r="K91" s="15"/>
+      <c r="L91" s="15"/>
+      <c r="M91" s="15"/>
+      <c r="N91" s="15"/>
+      <c r="T91" s="6"/>
     </row>
     <row r="92" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B92" s="23"/>
-      <c r="C92" s="18"/>
-      <c r="D92" s="7" t="s">
+      <c r="B92" s="29"/>
+      <c r="C92" s="9"/>
+      <c r="D92" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="K92" s="32"/>
-      <c r="L92" s="32"/>
-      <c r="M92" s="32"/>
-      <c r="N92" s="32"/>
-      <c r="T92" s="14"/>
+      <c r="K92" s="15"/>
+      <c r="L92" s="15"/>
+      <c r="M92" s="15"/>
+      <c r="N92" s="15"/>
+      <c r="T92" s="6"/>
     </row>
     <row r="93" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B93" s="23"/>
-      <c r="C93" s="18"/>
-      <c r="D93" s="7" t="s">
+      <c r="B93" s="29"/>
+      <c r="C93" s="9"/>
+      <c r="D93" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="K93" s="32"/>
-      <c r="L93" s="32"/>
-      <c r="M93" s="32"/>
-      <c r="N93" s="32"/>
-      <c r="T93" s="14"/>
+      <c r="K93" s="15"/>
+      <c r="L93" s="15"/>
+      <c r="M93" s="15"/>
+      <c r="N93" s="15"/>
+      <c r="T93" s="6"/>
     </row>
     <row r="94" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B94" s="23"/>
-      <c r="C94" s="18"/>
-      <c r="D94" s="7" t="s">
+      <c r="B94" s="29"/>
+      <c r="C94" s="9"/>
+      <c r="D94" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="K94" s="32"/>
-      <c r="L94" s="32"/>
-      <c r="M94" s="32"/>
-      <c r="N94" s="32"/>
-      <c r="T94" s="14"/>
+      <c r="K94" s="15"/>
+      <c r="L94" s="15"/>
+      <c r="M94" s="15"/>
+      <c r="N94" s="15"/>
+      <c r="T94" s="6"/>
     </row>
     <row r="95" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B95" s="23"/>
-      <c r="C95" s="18" t="s">
+      <c r="B95" s="29"/>
+      <c r="C95" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="D95" s="7" t="s">
+      <c r="D95" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="K95" s="32"/>
-      <c r="L95" s="32"/>
-      <c r="M95" s="32"/>
-      <c r="N95" s="32"/>
-      <c r="T95" s="14"/>
+      <c r="K95" s="15"/>
+      <c r="L95" s="15"/>
+      <c r="M95" s="15"/>
+      <c r="N95" s="15"/>
+      <c r="T95" s="6"/>
     </row>
     <row r="96" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B96" s="23"/>
-      <c r="C96" s="18"/>
-      <c r="D96" s="7" t="s">
+      <c r="B96" s="29"/>
+      <c r="C96" s="9"/>
+      <c r="D96" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="K96" s="32"/>
-      <c r="L96" s="32"/>
-      <c r="M96" s="32"/>
-      <c r="N96" s="32"/>
-      <c r="T96" s="14"/>
+      <c r="K96" s="15"/>
+      <c r="L96" s="15"/>
+      <c r="M96" s="15"/>
+      <c r="N96" s="15"/>
+      <c r="T96" s="6"/>
     </row>
     <row r="97" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B97" s="23"/>
-      <c r="C97" s="18"/>
-      <c r="D97" s="7" t="s">
+      <c r="B97" s="29"/>
+      <c r="C97" s="9"/>
+      <c r="D97" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="K97" s="32"/>
-      <c r="L97" s="32"/>
-      <c r="M97" s="32"/>
-      <c r="N97" s="32"/>
-      <c r="T97" s="14"/>
+      <c r="K97" s="15"/>
+      <c r="L97" s="15"/>
+      <c r="M97" s="15"/>
+      <c r="N97" s="15"/>
+      <c r="T97" s="6"/>
     </row>
     <row r="98" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B98" s="23"/>
-      <c r="C98" s="18"/>
-      <c r="D98" s="7" t="s">
+      <c r="B98" s="29"/>
+      <c r="C98" s="9"/>
+      <c r="D98" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="K98" s="32"/>
-      <c r="L98" s="32"/>
-      <c r="M98" s="32"/>
-      <c r="N98" s="32"/>
-      <c r="T98" s="14"/>
+      <c r="K98" s="15"/>
+      <c r="L98" s="15"/>
+      <c r="M98" s="15"/>
+      <c r="N98" s="15"/>
+      <c r="T98" s="6"/>
     </row>
     <row r="99" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B99" s="23"/>
-      <c r="C99" s="18"/>
-      <c r="D99" s="7" t="s">
+      <c r="B99" s="29"/>
+      <c r="C99" s="9"/>
+      <c r="D99" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="K99" s="32"/>
-      <c r="L99" s="32"/>
-      <c r="M99" s="32"/>
-      <c r="N99" s="32"/>
-      <c r="T99" s="14"/>
+      <c r="K99" s="15"/>
+      <c r="L99" s="15"/>
+      <c r="M99" s="15"/>
+      <c r="N99" s="15"/>
+      <c r="T99" s="6"/>
     </row>
     <row r="100" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B100" s="23"/>
-      <c r="C100" s="18"/>
-      <c r="D100" s="7" t="s">
+      <c r="B100" s="29"/>
+      <c r="C100" s="9"/>
+      <c r="D100" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="K100" s="32"/>
-      <c r="L100" s="32"/>
-      <c r="M100" s="32"/>
-      <c r="N100" s="32"/>
-      <c r="T100" s="14"/>
+      <c r="K100" s="15"/>
+      <c r="L100" s="15"/>
+      <c r="M100" s="15"/>
+      <c r="N100" s="15"/>
+      <c r="T100" s="6"/>
     </row>
     <row r="101" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B101" s="23"/>
-      <c r="C101" s="18"/>
-      <c r="D101" s="7" t="s">
+      <c r="B101" s="29"/>
+      <c r="C101" s="9"/>
+      <c r="D101" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="K101" s="32"/>
-      <c r="L101" s="32"/>
-      <c r="M101" s="32"/>
-      <c r="N101" s="32"/>
+      <c r="K101" s="15"/>
+      <c r="L101" s="15"/>
+      <c r="M101" s="15"/>
+      <c r="N101" s="15"/>
     </row>
     <row r="102" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B102" s="24"/>
-      <c r="C102" s="26" t="s">
+      <c r="B102" s="30"/>
+      <c r="C102" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="D102" s="27"/>
-      <c r="K102" s="32"/>
-      <c r="L102" s="32"/>
-      <c r="M102" s="32"/>
-      <c r="N102" s="32"/>
+      <c r="D102" s="32"/>
+      <c r="K102" s="15"/>
+      <c r="L102" s="15"/>
+      <c r="M102" s="15"/>
+      <c r="N102" s="15"/>
     </row>
     <row r="103" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B103" s="22" t="s">
+      <c r="B103" s="28" t="s">
         <v>177</v>
       </c>
-      <c r="C103" s="21" t="s">
+      <c r="C103" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D103" s="4" t="s">
+      <c r="D103" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="K103" s="32"/>
-      <c r="L103" s="32"/>
-      <c r="M103" s="32"/>
-      <c r="N103" s="32"/>
+      <c r="K103" s="15"/>
+      <c r="L103" s="15"/>
+      <c r="M103" s="15"/>
+      <c r="N103" s="15"/>
     </row>
     <row r="104" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B104" s="23"/>
-      <c r="C104" s="18"/>
-      <c r="D104" s="7" t="s">
+      <c r="B104" s="29"/>
+      <c r="C104" s="9"/>
+      <c r="D104" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="K104" s="32"/>
-      <c r="L104" s="32"/>
-      <c r="M104" s="32"/>
-      <c r="N104" s="32"/>
+      <c r="K104" s="15"/>
+      <c r="L104" s="15"/>
+      <c r="M104" s="15"/>
+      <c r="N104" s="15"/>
     </row>
     <row r="105" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B105" s="23"/>
-      <c r="C105" s="18"/>
-      <c r="D105" s="7" t="s">
+      <c r="B105" s="29"/>
+      <c r="C105" s="9"/>
+      <c r="D105" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="K105" s="32"/>
-      <c r="L105" s="32"/>
-      <c r="M105" s="32"/>
-      <c r="N105" s="32"/>
+      <c r="K105" s="15"/>
+      <c r="L105" s="15"/>
+      <c r="M105" s="15"/>
+      <c r="N105" s="15"/>
     </row>
     <row r="106" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B106" s="23"/>
-      <c r="C106" s="18"/>
-      <c r="D106" s="7" t="s">
+      <c r="B106" s="29"/>
+      <c r="C106" s="9"/>
+      <c r="D106" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="K106" s="32"/>
-      <c r="L106" s="32"/>
-      <c r="M106" s="32"/>
-      <c r="N106" s="32"/>
+      <c r="K106" s="15"/>
+      <c r="L106" s="15"/>
+      <c r="M106" s="15"/>
+      <c r="N106" s="15"/>
     </row>
     <row r="107" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B107" s="23"/>
-      <c r="C107" s="18"/>
-      <c r="D107" s="7" t="s">
+      <c r="B107" s="29"/>
+      <c r="C107" s="9"/>
+      <c r="D107" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="K107" s="32"/>
-      <c r="L107" s="32"/>
-      <c r="M107" s="32"/>
-      <c r="N107" s="32"/>
+      <c r="K107" s="15"/>
+      <c r="L107" s="15"/>
+      <c r="M107" s="15"/>
+      <c r="N107" s="15"/>
     </row>
     <row r="108" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B108" s="23"/>
-      <c r="C108" s="18"/>
-      <c r="D108" s="7" t="s">
+      <c r="B108" s="29"/>
+      <c r="C108" s="9"/>
+      <c r="D108" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="K108" s="32"/>
-      <c r="L108" s="32"/>
-      <c r="M108" s="32"/>
-      <c r="N108" s="32"/>
+      <c r="K108" s="15"/>
+      <c r="L108" s="15"/>
+      <c r="M108" s="15"/>
+      <c r="N108" s="15"/>
     </row>
     <row r="109" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B109" s="23"/>
-      <c r="C109" s="18"/>
-      <c r="D109" s="7" t="s">
+      <c r="B109" s="29"/>
+      <c r="C109" s="9"/>
+      <c r="D109" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="K109" s="32"/>
-      <c r="L109" s="32"/>
-      <c r="M109" s="32"/>
-      <c r="N109" s="32"/>
+      <c r="K109" s="15"/>
+      <c r="L109" s="15"/>
+      <c r="M109" s="15"/>
+      <c r="N109" s="15"/>
     </row>
     <row r="110" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B110" s="23"/>
-      <c r="C110" s="18"/>
-      <c r="D110" s="7" t="s">
+      <c r="B110" s="29"/>
+      <c r="C110" s="9"/>
+      <c r="D110" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="K110" s="32"/>
-      <c r="L110" s="32"/>
-      <c r="M110" s="32"/>
-      <c r="N110" s="32"/>
+      <c r="K110" s="15"/>
+      <c r="L110" s="15"/>
+      <c r="M110" s="15"/>
+      <c r="N110" s="15"/>
     </row>
     <row r="111" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B111" s="23"/>
-      <c r="C111" s="18"/>
-      <c r="D111" s="7" t="s">
+      <c r="B111" s="29"/>
+      <c r="C111" s="9"/>
+      <c r="D111" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="K111" s="32"/>
-      <c r="L111" s="32"/>
-      <c r="M111" s="32"/>
-      <c r="N111" s="32"/>
+      <c r="K111" s="15"/>
+      <c r="L111" s="15"/>
+      <c r="M111" s="15"/>
+      <c r="N111" s="15"/>
     </row>
     <row r="112" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B112" s="23"/>
-      <c r="C112" s="18"/>
-      <c r="D112" s="7" t="s">
+      <c r="B112" s="29"/>
+      <c r="C112" s="9"/>
+      <c r="D112" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="K112" s="32"/>
-      <c r="L112" s="32"/>
-      <c r="M112" s="32"/>
-      <c r="N112" s="32"/>
+      <c r="K112" s="15"/>
+      <c r="L112" s="15"/>
+      <c r="M112" s="15"/>
+      <c r="N112" s="15"/>
     </row>
     <row r="113" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B113" s="23"/>
-      <c r="C113" s="18"/>
-      <c r="D113" s="7" t="s">
+      <c r="B113" s="29"/>
+      <c r="C113" s="9"/>
+      <c r="D113" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="K113" s="32"/>
-      <c r="L113" s="32"/>
-      <c r="M113" s="32"/>
-      <c r="N113" s="32"/>
+      <c r="K113" s="15"/>
+      <c r="L113" s="15"/>
+      <c r="M113" s="15"/>
+      <c r="N113" s="15"/>
     </row>
     <row r="114" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B114" s="23"/>
-      <c r="C114" s="18" t="s">
+      <c r="B114" s="29"/>
+      <c r="C114" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D114" s="7" t="s">
+      <c r="D114" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="K114" s="32"/>
-      <c r="L114" s="32"/>
-      <c r="M114" s="32"/>
-      <c r="N114" s="32"/>
+      <c r="K114" s="15"/>
+      <c r="L114" s="15"/>
+      <c r="M114" s="15"/>
+      <c r="N114" s="15"/>
     </row>
     <row r="115" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B115" s="23"/>
-      <c r="C115" s="18"/>
-      <c r="D115" s="7" t="s">
+      <c r="B115" s="29"/>
+      <c r="C115" s="9"/>
+      <c r="D115" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="K115" s="32"/>
-      <c r="L115" s="32"/>
-      <c r="M115" s="32"/>
-      <c r="N115" s="32"/>
+      <c r="K115" s="15"/>
+      <c r="L115" s="15"/>
+      <c r="M115" s="15"/>
+      <c r="N115" s="15"/>
     </row>
     <row r="116" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B116" s="23"/>
-      <c r="C116" s="18"/>
-      <c r="D116" s="7" t="s">
+      <c r="B116" s="29"/>
+      <c r="C116" s="9"/>
+      <c r="D116" s="3" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="117" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B117" s="23"/>
-      <c r="C117" s="18"/>
-      <c r="D117" s="7" t="s">
+      <c r="B117" s="29"/>
+      <c r="C117" s="9"/>
+      <c r="D117" s="3" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="118" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B118" s="23"/>
-      <c r="C118" s="18"/>
-      <c r="D118" s="7" t="s">
+      <c r="B118" s="29"/>
+      <c r="C118" s="9"/>
+      <c r="D118" s="3" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="119" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B119" s="23"/>
-      <c r="C119" s="18"/>
-      <c r="D119" s="7" t="s">
+      <c r="B119" s="29"/>
+      <c r="C119" s="9"/>
+      <c r="D119" s="3" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="120" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B120" s="23"/>
-      <c r="C120" s="18"/>
-      <c r="D120" s="7" t="s">
+      <c r="B120" s="29"/>
+      <c r="C120" s="9"/>
+      <c r="D120" s="3" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="121" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B121" s="23"/>
-      <c r="C121" s="18"/>
-      <c r="D121" s="7" t="s">
+      <c r="B121" s="29"/>
+      <c r="C121" s="9"/>
+      <c r="D121" s="3" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="122" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B122" s="23"/>
-      <c r="C122" s="18"/>
-      <c r="D122" s="7" t="s">
+      <c r="B122" s="29"/>
+      <c r="C122" s="9"/>
+      <c r="D122" s="3" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="123" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B123" s="23"/>
-      <c r="C123" s="18"/>
-      <c r="D123" s="7" t="s">
+      <c r="B123" s="29"/>
+      <c r="C123" s="9"/>
+      <c r="D123" s="3" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="124" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B124" s="23"/>
-      <c r="C124" s="18" t="s">
+      <c r="B124" s="29"/>
+      <c r="C124" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D124" s="7" t="s">
+      <c r="D124" s="3" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="125" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B125" s="23"/>
-      <c r="C125" s="18"/>
-      <c r="D125" s="7" t="s">
+      <c r="B125" s="29"/>
+      <c r="C125" s="9"/>
+      <c r="D125" s="3" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="126" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B126" s="23"/>
-      <c r="C126" s="18"/>
-      <c r="D126" s="7" t="s">
+      <c r="B126" s="29"/>
+      <c r="C126" s="9"/>
+      <c r="D126" s="3" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="127" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B127" s="23"/>
-      <c r="C127" s="18"/>
-      <c r="D127" s="7" t="s">
+      <c r="B127" s="29"/>
+      <c r="C127" s="9"/>
+      <c r="D127" s="3" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="128" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B128" s="23"/>
-      <c r="C128" s="18"/>
-      <c r="D128" s="7" t="s">
+      <c r="B128" s="29"/>
+      <c r="C128" s="9"/>
+      <c r="D128" s="3" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="129" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B129" s="23"/>
-      <c r="C129" s="18"/>
-      <c r="D129" s="7" t="s">
+      <c r="B129" s="29"/>
+      <c r="C129" s="9"/>
+      <c r="D129" s="3" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="130" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B130" s="23"/>
-      <c r="C130" s="18"/>
-      <c r="D130" s="7" t="s">
+      <c r="B130" s="29"/>
+      <c r="C130" s="9"/>
+      <c r="D130" s="3" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="131" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B131" s="23"/>
-      <c r="C131" s="18"/>
-      <c r="D131" s="7" t="s">
+      <c r="B131" s="29"/>
+      <c r="C131" s="9"/>
+      <c r="D131" s="3" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="132" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B132" s="23"/>
-      <c r="C132" s="18"/>
-      <c r="D132" s="7" t="s">
+      <c r="B132" s="29"/>
+      <c r="C132" s="9"/>
+      <c r="D132" s="3" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="133" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B133" s="23"/>
-      <c r="C133" s="18"/>
-      <c r="D133" s="7" t="s">
+      <c r="B133" s="29"/>
+      <c r="C133" s="9"/>
+      <c r="D133" s="3" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="134" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B134" s="23"/>
-      <c r="C134" s="18"/>
-      <c r="D134" s="7" t="s">
+      <c r="B134" s="29"/>
+      <c r="C134" s="9"/>
+      <c r="D134" s="3" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="135" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B135" s="23"/>
-      <c r="C135" s="18"/>
-      <c r="D135" s="7" t="s">
+      <c r="B135" s="29"/>
+      <c r="C135" s="9"/>
+      <c r="D135" s="3" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="136" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B136" s="23"/>
-      <c r="C136" s="18" t="s">
+      <c r="B136" s="29"/>
+      <c r="C136" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D136" s="7" t="s">
+      <c r="D136" s="3" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="137" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B137" s="23"/>
-      <c r="C137" s="18"/>
-      <c r="D137" s="7" t="s">
+      <c r="B137" s="29"/>
+      <c r="C137" s="9"/>
+      <c r="D137" s="3" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="138" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B138" s="23"/>
-      <c r="C138" s="18"/>
-      <c r="D138" s="7" t="s">
+      <c r="B138" s="29"/>
+      <c r="C138" s="9"/>
+      <c r="D138" s="3" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="139" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B139" s="23"/>
-      <c r="C139" s="18"/>
-      <c r="D139" s="7" t="s">
+      <c r="B139" s="29"/>
+      <c r="C139" s="9"/>
+      <c r="D139" s="3" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="140" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B140" s="23"/>
-      <c r="C140" s="18"/>
-      <c r="D140" s="7" t="s">
+      <c r="B140" s="29"/>
+      <c r="C140" s="9"/>
+      <c r="D140" s="3" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="141" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B141" s="23"/>
-      <c r="C141" s="18"/>
-      <c r="D141" s="7" t="s">
+      <c r="B141" s="29"/>
+      <c r="C141" s="9"/>
+      <c r="D141" s="3" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="142" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B142" s="23"/>
-      <c r="C142" s="18"/>
-      <c r="D142" s="7" t="s">
+      <c r="B142" s="29"/>
+      <c r="C142" s="9"/>
+      <c r="D142" s="3" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="143" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B143" s="23"/>
-      <c r="C143" s="18"/>
-      <c r="D143" s="7" t="s">
+      <c r="B143" s="29"/>
+      <c r="C143" s="9"/>
+      <c r="D143" s="3" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="144" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B144" s="23"/>
-      <c r="C144" s="18"/>
-      <c r="D144" s="7" t="s">
+      <c r="B144" s="29"/>
+      <c r="C144" s="9"/>
+      <c r="D144" s="3" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="145" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B145" s="23"/>
-      <c r="C145" s="18"/>
-      <c r="D145" s="7" t="s">
+      <c r="B145" s="29"/>
+      <c r="C145" s="9"/>
+      <c r="D145" s="3" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="146" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B146" s="23"/>
-      <c r="C146" s="18"/>
-      <c r="D146" s="7" t="s">
+      <c r="B146" s="29"/>
+      <c r="C146" s="9"/>
+      <c r="D146" s="3" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="147" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B147" s="23"/>
-      <c r="C147" s="18" t="s">
+      <c r="B147" s="29"/>
+      <c r="C147" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D147" s="7" t="s">
+      <c r="D147" s="3" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="148" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B148" s="23"/>
-      <c r="C148" s="18"/>
-      <c r="D148" s="7" t="s">
+      <c r="B148" s="29"/>
+      <c r="C148" s="9"/>
+      <c r="D148" s="3" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="149" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B149" s="23"/>
-      <c r="C149" s="18"/>
-      <c r="D149" s="7" t="s">
+      <c r="B149" s="29"/>
+      <c r="C149" s="9"/>
+      <c r="D149" s="3" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="150" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B150" s="23"/>
-      <c r="C150" s="18"/>
-      <c r="D150" s="7" t="s">
+      <c r="B150" s="29"/>
+      <c r="C150" s="9"/>
+      <c r="D150" s="3" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="151" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B151" s="23"/>
-      <c r="C151" s="18"/>
-      <c r="D151" s="7" t="s">
+      <c r="B151" s="29"/>
+      <c r="C151" s="9"/>
+      <c r="D151" s="3" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="152" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B152" s="23"/>
-      <c r="C152" s="18"/>
-      <c r="D152" s="7" t="s">
+      <c r="B152" s="29"/>
+      <c r="C152" s="9"/>
+      <c r="D152" s="3" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="153" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B153" s="23"/>
-      <c r="C153" s="18"/>
-      <c r="D153" s="7" t="s">
+      <c r="B153" s="29"/>
+      <c r="C153" s="9"/>
+      <c r="D153" s="3" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="154" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B154" s="23"/>
-      <c r="C154" s="18" t="s">
+      <c r="B154" s="29"/>
+      <c r="C154" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D154" s="7" t="s">
+      <c r="D154" s="3" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="155" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B155" s="23"/>
-      <c r="C155" s="18"/>
-      <c r="D155" s="7" t="s">
+      <c r="B155" s="29"/>
+      <c r="C155" s="9"/>
+      <c r="D155" s="3" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="156" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B156" s="23"/>
-      <c r="C156" s="18"/>
-      <c r="D156" s="7" t="s">
+      <c r="B156" s="29"/>
+      <c r="C156" s="9"/>
+      <c r="D156" s="3" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="157" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B157" s="23"/>
-      <c r="C157" s="18"/>
-      <c r="D157" s="7" t="s">
+      <c r="B157" s="29"/>
+      <c r="C157" s="9"/>
+      <c r="D157" s="3" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="158" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B158" s="23"/>
-      <c r="C158" s="18"/>
-      <c r="D158" s="7" t="s">
+      <c r="B158" s="29"/>
+      <c r="C158" s="9"/>
+      <c r="D158" s="3" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="159" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B159" s="23"/>
-      <c r="C159" s="18"/>
-      <c r="D159" s="7" t="s">
+      <c r="B159" s="29"/>
+      <c r="C159" s="9"/>
+      <c r="D159" s="3" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="160" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B160" s="23"/>
-      <c r="C160" s="18" t="s">
+      <c r="B160" s="29"/>
+      <c r="C160" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="D160" s="7" t="s">
+      <c r="D160" s="3" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="161" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B161" s="23"/>
-      <c r="C161" s="18"/>
-      <c r="D161" s="7" t="s">
+      <c r="B161" s="29"/>
+      <c r="C161" s="9"/>
+      <c r="D161" s="3" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="162" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B162" s="23"/>
-      <c r="C162" s="20" t="s">
+      <c r="B162" s="29"/>
+      <c r="C162" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="D162" s="19"/>
+      <c r="D162" s="10"/>
     </row>
     <row r="163" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B163" s="2" t="s">
+      <c r="B163" s="21" t="s">
         <v>238</v>
       </c>
-      <c r="C163" s="3" t="s">
+      <c r="C163" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="D163" s="4" t="s">
+      <c r="D163" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="164" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B164" s="5"/>
-      <c r="C164" s="6"/>
-      <c r="D164" s="7" t="s">
+      <c r="B164" s="22"/>
+      <c r="C164" s="18"/>
+      <c r="D164" s="3" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="165" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B165" s="5"/>
-      <c r="C165" s="6"/>
-      <c r="D165" s="7" t="s">
+      <c r="B165" s="22"/>
+      <c r="C165" s="18"/>
+      <c r="D165" s="3" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="166" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B166" s="5"/>
-      <c r="C166" s="6"/>
-      <c r="D166" s="7" t="s">
+      <c r="B166" s="22"/>
+      <c r="C166" s="18"/>
+      <c r="D166" s="3" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="167" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B167" s="5"/>
-      <c r="C167" s="6"/>
-      <c r="D167" s="7" t="s">
+      <c r="B167" s="22"/>
+      <c r="C167" s="18"/>
+      <c r="D167" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="168" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B168" s="5"/>
-      <c r="C168" s="6" t="s">
+      <c r="B168" s="22"/>
+      <c r="C168" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D168" s="7" t="s">
+      <c r="D168" s="3" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="169" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B169" s="5"/>
-      <c r="C169" s="6"/>
-      <c r="D169" s="7" t="s">
+      <c r="B169" s="22"/>
+      <c r="C169" s="18"/>
+      <c r="D169" s="3" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="170" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B170" s="5"/>
-      <c r="C170" s="6"/>
-      <c r="D170" s="7" t="s">
+      <c r="B170" s="22"/>
+      <c r="C170" s="18"/>
+      <c r="D170" s="3" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="171" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B171" s="5"/>
-      <c r="C171" s="6"/>
-      <c r="D171" s="7" t="s">
+      <c r="B171" s="22"/>
+      <c r="C171" s="18"/>
+      <c r="D171" s="3" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="172" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B172" s="5"/>
-      <c r="C172" s="6"/>
-      <c r="D172" s="7" t="s">
+      <c r="B172" s="22"/>
+      <c r="C172" s="18"/>
+      <c r="D172" s="3" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="173" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B173" s="5"/>
-      <c r="C173" s="6"/>
-      <c r="D173" s="7" t="s">
+      <c r="B173" s="22"/>
+      <c r="C173" s="18"/>
+      <c r="D173" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="174" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B174" s="5"/>
-      <c r="C174" s="6" t="s">
+      <c r="B174" s="22"/>
+      <c r="C174" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D174" s="7" t="s">
+      <c r="D174" s="3" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="175" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B175" s="5"/>
-      <c r="C175" s="6"/>
-      <c r="D175" s="7" t="s">
+      <c r="B175" s="22"/>
+      <c r="C175" s="18"/>
+      <c r="D175" s="3" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="176" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B176" s="5"/>
-      <c r="C176" s="6"/>
-      <c r="D176" s="7" t="s">
+      <c r="B176" s="22"/>
+      <c r="C176" s="18"/>
+      <c r="D176" s="3" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="177" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B177" s="5"/>
-      <c r="C177" s="6"/>
-      <c r="D177" s="7" t="s">
+      <c r="B177" s="22"/>
+      <c r="C177" s="18"/>
+      <c r="D177" s="3" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="178" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B178" s="5"/>
-      <c r="C178" s="6"/>
-      <c r="D178" s="7" t="s">
+      <c r="B178" s="22"/>
+      <c r="C178" s="18"/>
+      <c r="D178" s="3" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="179" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B179" s="5"/>
-      <c r="C179" s="6"/>
-      <c r="D179" s="7" t="s">
+      <c r="B179" s="22"/>
+      <c r="C179" s="18"/>
+      <c r="D179" s="3" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="180" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B180" s="5"/>
-      <c r="C180" s="6"/>
-      <c r="D180" s="7" t="s">
+      <c r="B180" s="22"/>
+      <c r="C180" s="18"/>
+      <c r="D180" s="3" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="181" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B181" s="5"/>
-      <c r="C181" s="6"/>
-      <c r="D181" s="7" t="s">
+      <c r="B181" s="22"/>
+      <c r="C181" s="18"/>
+      <c r="D181" s="3" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="182" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B182" s="5"/>
-      <c r="C182" s="6"/>
-      <c r="D182" s="7" t="s">
+      <c r="B182" s="22"/>
+      <c r="C182" s="18"/>
+      <c r="D182" s="3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="183" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B183" s="5"/>
-      <c r="C183" s="6" t="s">
+      <c r="B183" s="22"/>
+      <c r="C183" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="D183" s="7" t="s">
+      <c r="D183" s="3" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="184" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B184" s="5"/>
-      <c r="C184" s="6"/>
-      <c r="D184" s="7" t="s">
+      <c r="B184" s="22"/>
+      <c r="C184" s="18"/>
+      <c r="D184" s="3" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="185" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B185" s="5"/>
-      <c r="C185" s="6"/>
-      <c r="D185" s="7" t="s">
+      <c r="B185" s="22"/>
+      <c r="C185" s="18"/>
+      <c r="D185" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="186" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B186" s="5"/>
-      <c r="C186" s="6"/>
-      <c r="D186" s="7" t="s">
+      <c r="B186" s="22"/>
+      <c r="C186" s="18"/>
+      <c r="D186" s="3" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="187" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B187" s="5"/>
-      <c r="C187" s="6"/>
-      <c r="D187" s="7" t="s">
+      <c r="B187" s="22"/>
+      <c r="C187" s="18"/>
+      <c r="D187" s="3" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="188" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B188" s="5"/>
-      <c r="C188" s="6"/>
-      <c r="D188" s="7" t="s">
+      <c r="B188" s="22"/>
+      <c r="C188" s="18"/>
+      <c r="D188" s="3" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="189" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B189" s="5"/>
-      <c r="C189" s="6"/>
-      <c r="D189" s="7" t="s">
+      <c r="B189" s="22"/>
+      <c r="C189" s="18"/>
+      <c r="D189" s="3" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="190" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B190" s="5"/>
-      <c r="C190" s="6" t="s">
+      <c r="B190" s="22"/>
+      <c r="C190" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="D190" s="7" t="s">
+      <c r="D190" s="3" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="191" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B191" s="5"/>
-      <c r="C191" s="6"/>
-      <c r="D191" s="7" t="s">
+      <c r="B191" s="22"/>
+      <c r="C191" s="18"/>
+      <c r="D191" s="3" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="192" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B192" s="5"/>
-      <c r="C192" s="6"/>
-      <c r="D192" s="7" t="s">
+      <c r="B192" s="22"/>
+      <c r="C192" s="18"/>
+      <c r="D192" s="3" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="193" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B193" s="5"/>
-      <c r="C193" s="6"/>
-      <c r="D193" s="7" t="s">
+      <c r="B193" s="22"/>
+      <c r="C193" s="18"/>
+      <c r="D193" s="3" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="194" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B194" s="5"/>
-      <c r="C194" s="6"/>
-      <c r="D194" s="7" t="s">
+      <c r="B194" s="22"/>
+      <c r="C194" s="18"/>
+      <c r="D194" s="3" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="195" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B195" s="5"/>
-      <c r="C195" s="6"/>
-      <c r="D195" s="7" t="s">
+      <c r="B195" s="22"/>
+      <c r="C195" s="18"/>
+      <c r="D195" s="3" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="196" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B196" s="5"/>
-      <c r="C196" s="6"/>
-      <c r="D196" s="7" t="s">
+      <c r="B196" s="22"/>
+      <c r="C196" s="18"/>
+      <c r="D196" s="3" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="197" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B197" s="5"/>
-      <c r="C197" s="6"/>
-      <c r="D197" s="7" t="s">
+      <c r="B197" s="22"/>
+      <c r="C197" s="18"/>
+      <c r="D197" s="3" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="198" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B198" s="5"/>
-      <c r="C198" s="6"/>
-      <c r="D198" s="7" t="s">
+      <c r="B198" s="22"/>
+      <c r="C198" s="18"/>
+      <c r="D198" s="3" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="199" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B199" s="5"/>
-      <c r="C199" s="6" t="s">
+      <c r="B199" s="22"/>
+      <c r="C199" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D199" s="7" t="s">
+      <c r="D199" s="3" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="200" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B200" s="5"/>
-      <c r="C200" s="6"/>
-      <c r="D200" s="7" t="s">
+      <c r="B200" s="22"/>
+      <c r="C200" s="18"/>
+      <c r="D200" s="3" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="201" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B201" s="5"/>
-      <c r="C201" s="6"/>
-      <c r="D201" s="7" t="s">
+      <c r="B201" s="22"/>
+      <c r="C201" s="18"/>
+      <c r="D201" s="3" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="202" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B202" s="5"/>
-      <c r="C202" s="6"/>
-      <c r="D202" s="7" t="s">
+      <c r="B202" s="22"/>
+      <c r="C202" s="18"/>
+      <c r="D202" s="3" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="203" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B203" s="5"/>
-      <c r="C203" s="6"/>
-      <c r="D203" s="7" t="s">
+      <c r="B203" s="22"/>
+      <c r="C203" s="18"/>
+      <c r="D203" s="3" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="204" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B204" s="5"/>
-      <c r="C204" s="6"/>
-      <c r="D204" s="7" t="s">
+      <c r="B204" s="22"/>
+      <c r="C204" s="18"/>
+      <c r="D204" s="3" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="205" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B205" s="5"/>
-      <c r="C205" s="6" t="s">
+      <c r="B205" s="22"/>
+      <c r="C205" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="D205" s="7" t="s">
+      <c r="D205" s="3" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="206" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B206" s="5"/>
-      <c r="C206" s="6"/>
-      <c r="D206" s="7" t="s">
+      <c r="B206" s="22"/>
+      <c r="C206" s="18"/>
+      <c r="D206" s="3" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="207" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B207" s="5"/>
-      <c r="C207" s="6"/>
-      <c r="D207" s="7" t="s">
+      <c r="B207" s="22"/>
+      <c r="C207" s="18"/>
+      <c r="D207" s="3" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="208" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B208" s="5"/>
-      <c r="C208" s="6"/>
-      <c r="D208" s="7" t="s">
+      <c r="B208" s="22"/>
+      <c r="C208" s="18"/>
+      <c r="D208" s="3" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="209" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B209" s="5"/>
-      <c r="C209" s="6"/>
-      <c r="D209" s="7" t="s">
+      <c r="B209" s="22"/>
+      <c r="C209" s="18"/>
+      <c r="D209" s="3" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="210" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B210" s="5"/>
-      <c r="C210" s="6"/>
-      <c r="D210" s="7" t="s">
+      <c r="B210" s="22"/>
+      <c r="C210" s="18"/>
+      <c r="D210" s="3" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="211" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B211" s="5"/>
-      <c r="C211" s="6"/>
-      <c r="D211" s="7" t="s">
+      <c r="B211" s="22"/>
+      <c r="C211" s="18"/>
+      <c r="D211" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="212" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B212" s="5"/>
-      <c r="C212" s="6" t="s">
+      <c r="B212" s="22"/>
+      <c r="C212" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="D212" s="7" t="s">
+      <c r="D212" s="3" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="213" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B213" s="5"/>
-      <c r="C213" s="6"/>
-      <c r="D213" s="7" t="s">
+      <c r="B213" s="22"/>
+      <c r="C213" s="18"/>
+      <c r="D213" s="3" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="214" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B214" s="5"/>
-      <c r="C214" s="6"/>
-      <c r="D214" s="7" t="s">
+      <c r="B214" s="22"/>
+      <c r="C214" s="18"/>
+      <c r="D214" s="3" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="215" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B215" s="5"/>
-      <c r="C215" s="6"/>
-      <c r="D215" s="7" t="s">
+      <c r="B215" s="22"/>
+      <c r="C215" s="18"/>
+      <c r="D215" s="3" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="216" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B216" s="5"/>
-      <c r="C216" s="6"/>
-      <c r="D216" s="7" t="s">
+      <c r="B216" s="22"/>
+      <c r="C216" s="18"/>
+      <c r="D216" s="3" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="217" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B217" s="5"/>
-      <c r="C217" s="6"/>
-      <c r="D217" s="7" t="s">
+      <c r="B217" s="22"/>
+      <c r="C217" s="18"/>
+      <c r="D217" s="3" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="218" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B218" s="5"/>
-      <c r="C218" s="6" t="s">
+      <c r="B218" s="22"/>
+      <c r="C218" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="D218" s="7" t="s">
+      <c r="D218" s="3" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="219" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B219" s="5"/>
-      <c r="C219" s="6"/>
-      <c r="D219" s="7" t="s">
+      <c r="B219" s="22"/>
+      <c r="C219" s="18"/>
+      <c r="D219" s="3" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="220" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B220" s="5"/>
-      <c r="C220" s="6"/>
-      <c r="D220" s="7" t="s">
+      <c r="B220" s="22"/>
+      <c r="C220" s="18"/>
+      <c r="D220" s="3" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="221" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B221" s="8"/>
-      <c r="C221" s="9"/>
-      <c r="D221" s="17" t="s">
+      <c r="B221" s="23"/>
+      <c r="C221" s="19"/>
+      <c r="D221" s="8" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="222" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B222" s="2" t="s">
+      <c r="B222" s="21" t="s">
         <v>237</v>
       </c>
-      <c r="C222" s="3" t="s">
+      <c r="C222" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="D222" s="4" t="s">
+      <c r="D222" s="2" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="223" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B223" s="5"/>
-      <c r="C223" s="6"/>
-      <c r="D223" s="7" t="s">
+      <c r="B223" s="22"/>
+      <c r="C223" s="18"/>
+      <c r="D223" s="3" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="224" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B224" s="5"/>
-      <c r="C224" s="6"/>
-      <c r="D224" s="7" t="s">
+      <c r="B224" s="22"/>
+      <c r="C224" s="18"/>
+      <c r="D224" s="3" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="225" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B225" s="5"/>
-      <c r="C225" s="6" t="s">
+      <c r="B225" s="22"/>
+      <c r="C225" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D225" s="7" t="s">
+      <c r="D225" s="3" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="226" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B226" s="5"/>
-      <c r="C226" s="6"/>
-      <c r="D226" s="7" t="s">
+      <c r="B226" s="22"/>
+      <c r="C226" s="18"/>
+      <c r="D226" s="3" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="227" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B227" s="5"/>
-      <c r="C227" s="6"/>
-      <c r="D227" s="7" t="s">
+      <c r="B227" s="22"/>
+      <c r="C227" s="18"/>
+      <c r="D227" s="3" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="228" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B228" s="5"/>
-      <c r="C228" s="6"/>
-      <c r="D228" s="7" t="s">
+      <c r="B228" s="22"/>
+      <c r="C228" s="18"/>
+      <c r="D228" s="3" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="229" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B229" s="5"/>
-      <c r="C229" s="6"/>
-      <c r="D229" s="7" t="s">
+      <c r="B229" s="22"/>
+      <c r="C229" s="18"/>
+      <c r="D229" s="3" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="230" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B230" s="5"/>
-      <c r="C230" s="6" t="s">
+      <c r="B230" s="22"/>
+      <c r="C230" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D230" s="7" t="s">
+      <c r="D230" s="3" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="231" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B231" s="5"/>
-      <c r="C231" s="6"/>
-      <c r="D231" s="7" t="s">
+      <c r="B231" s="22"/>
+      <c r="C231" s="18"/>
+      <c r="D231" s="3" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="232" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B232" s="5"/>
-      <c r="C232" s="6" t="s">
+      <c r="B232" s="22"/>
+      <c r="C232" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="D232" s="7" t="s">
+      <c r="D232" s="3" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="233" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B233" s="5"/>
-      <c r="C233" s="6"/>
-      <c r="D233" s="7" t="s">
+      <c r="B233" s="22"/>
+      <c r="C233" s="18"/>
+      <c r="D233" s="3" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="234" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B234" s="5"/>
-      <c r="C234" s="6"/>
-      <c r="D234" s="7" t="s">
+      <c r="B234" s="22"/>
+      <c r="C234" s="18"/>
+      <c r="D234" s="3" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="235" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B235" s="5"/>
-      <c r="C235" s="18" t="s">
+      <c r="B235" s="22"/>
+      <c r="C235" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D235" s="7" t="s">
+      <c r="D235" s="3" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="236" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B236" s="5"/>
-      <c r="C236" s="18" t="s">
+      <c r="B236" s="22"/>
+      <c r="C236" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D236" s="7" t="s">
+      <c r="D236" s="3" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="237" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B237" s="5"/>
-      <c r="C237" s="18" t="s">
+      <c r="B237" s="22"/>
+      <c r="C237" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="D237" s="7" t="s">
+      <c r="D237" s="3" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="238" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B238" s="5"/>
-      <c r="C238" s="6" t="s">
+      <c r="B238" s="22"/>
+      <c r="C238" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="D238" s="7" t="s">
+      <c r="D238" s="3" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="239" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B239" s="5"/>
-      <c r="C239" s="6"/>
-      <c r="D239" s="7" t="s">
+      <c r="B239" s="22"/>
+      <c r="C239" s="18"/>
+      <c r="D239" s="3" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="240" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B240" s="5"/>
-      <c r="C240" s="6"/>
-      <c r="D240" s="7" t="s">
+      <c r="B240" s="22"/>
+      <c r="C240" s="18"/>
+      <c r="D240" s="3" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="241" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B241" s="5"/>
-      <c r="C241" s="6"/>
-      <c r="D241" s="7" t="s">
+      <c r="B241" s="22"/>
+      <c r="C241" s="18"/>
+      <c r="D241" s="3" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="242" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B242" s="5"/>
-      <c r="C242" s="6" t="s">
+      <c r="B242" s="22"/>
+      <c r="C242" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="D242" s="7" t="s">
+      <c r="D242" s="3" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="243" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B243" s="5"/>
-      <c r="C243" s="6"/>
-      <c r="D243" s="7" t="s">
+      <c r="B243" s="22"/>
+      <c r="C243" s="18"/>
+      <c r="D243" s="3" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="244" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B244" s="5"/>
-      <c r="C244" s="6"/>
-      <c r="D244" s="7" t="s">
+      <c r="B244" s="22"/>
+      <c r="C244" s="18"/>
+      <c r="D244" s="3" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="245" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B245" s="5"/>
-      <c r="C245" s="6"/>
-      <c r="D245" s="7" t="s">
+      <c r="B245" s="22"/>
+      <c r="C245" s="18"/>
+      <c r="D245" s="3" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="246" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B246" s="5"/>
-      <c r="C246" s="6"/>
-      <c r="D246" s="7" t="s">
+      <c r="B246" s="22"/>
+      <c r="C246" s="18"/>
+      <c r="D246" s="3" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="247" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B247" s="5"/>
-      <c r="C247" s="6"/>
-      <c r="D247" s="7" t="s">
+      <c r="B247" s="22"/>
+      <c r="C247" s="18"/>
+      <c r="D247" s="3" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="248" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B248" s="5"/>
-      <c r="C248" s="18" t="s">
+      <c r="B248" s="22"/>
+      <c r="C248" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="D248" s="7" t="s">
+      <c r="D248" s="3" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="249" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B249" s="5"/>
-      <c r="C249" s="6" t="s">
+      <c r="B249" s="22"/>
+      <c r="C249" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="D249" s="7" t="s">
+      <c r="D249" s="3" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="250" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B250" s="5"/>
-      <c r="C250" s="6"/>
-      <c r="D250" s="7" t="s">
+      <c r="B250" s="22"/>
+      <c r="C250" s="18"/>
+      <c r="D250" s="3" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="251" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B251" s="5"/>
-      <c r="C251" s="18" t="s">
+      <c r="B251" s="22"/>
+      <c r="C251" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="D251" s="7" t="s">
+      <c r="D251" s="3" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="252" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B252" s="5"/>
-      <c r="C252" s="6" t="s">
+      <c r="B252" s="22"/>
+      <c r="C252" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="D252" s="7" t="s">
+      <c r="D252" s="3" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="253" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B253" s="5"/>
-      <c r="C253" s="6"/>
-      <c r="D253" s="7" t="s">
+      <c r="B253" s="22"/>
+      <c r="C253" s="18"/>
+      <c r="D253" s="3" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="254" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B254" s="5"/>
-      <c r="C254" s="6" t="s">
+      <c r="B254" s="22"/>
+      <c r="C254" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="D254" s="7" t="s">
+      <c r="D254" s="3" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="255" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B255" s="5"/>
-      <c r="C255" s="6"/>
-      <c r="D255" s="7" t="s">
+      <c r="B255" s="22"/>
+      <c r="C255" s="18"/>
+      <c r="D255" s="3" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="256" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B256" s="5"/>
-      <c r="C256" s="6"/>
-      <c r="D256" s="7" t="s">
+      <c r="B256" s="22"/>
+      <c r="C256" s="18"/>
+      <c r="D256" s="3" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="257" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B257" s="5"/>
-      <c r="C257" s="6"/>
-      <c r="D257" s="7" t="s">
+      <c r="B257" s="22"/>
+      <c r="C257" s="18"/>
+      <c r="D257" s="3" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="258" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B258" s="5"/>
-      <c r="C258" s="6"/>
-      <c r="D258" s="7" t="s">
+      <c r="B258" s="22"/>
+      <c r="C258" s="18"/>
+      <c r="D258" s="3" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="259" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B259" s="5"/>
-      <c r="C259" s="18" t="s">
+      <c r="B259" s="22"/>
+      <c r="C259" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="D259" s="7" t="s">
+      <c r="D259" s="3" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="260" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B260" s="5"/>
-      <c r="C260" s="18" t="s">
+      <c r="B260" s="22"/>
+      <c r="C260" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="D260" s="7" t="s">
+      <c r="D260" s="3" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="261" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B261" s="5"/>
-      <c r="C261" s="6" t="s">
+      <c r="B261" s="22"/>
+      <c r="C261" s="18" t="s">
         <v>279</v>
       </c>
-      <c r="D261" s="7" t="s">
+      <c r="D261" s="3" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="262" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B262" s="5"/>
-      <c r="C262" s="6"/>
-      <c r="D262" s="7" t="s">
+      <c r="B262" s="22"/>
+      <c r="C262" s="18"/>
+      <c r="D262" s="3" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="263" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B263" s="5"/>
-      <c r="C263" s="6" t="s">
+      <c r="B263" s="22"/>
+      <c r="C263" s="18" t="s">
         <v>282</v>
       </c>
-      <c r="D263" s="7" t="s">
+      <c r="D263" s="3" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="264" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B264" s="5"/>
-      <c r="C264" s="6"/>
-      <c r="D264" s="7" t="s">
+      <c r="B264" s="22"/>
+      <c r="C264" s="18"/>
+      <c r="D264" s="3" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="265" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B265" s="5"/>
-      <c r="C265" s="6"/>
-      <c r="D265" s="7" t="s">
+      <c r="B265" s="22"/>
+      <c r="C265" s="18"/>
+      <c r="D265" s="3" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="266" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B266" s="5"/>
-      <c r="C266" s="6" t="s">
+      <c r="B266" s="22"/>
+      <c r="C266" s="18" t="s">
         <v>287</v>
       </c>
-      <c r="D266" s="7" t="s">
+      <c r="D266" s="3" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="267" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B267" s="5"/>
-      <c r="C267" s="6"/>
-      <c r="D267" s="7" t="s">
+      <c r="B267" s="22"/>
+      <c r="C267" s="18"/>
+      <c r="D267" s="3" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="268" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B268" s="5"/>
-      <c r="C268" s="6"/>
-      <c r="D268" s="7" t="s">
+      <c r="B268" s="22"/>
+      <c r="C268" s="18"/>
+      <c r="D268" s="3" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="269" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B269" s="5"/>
-      <c r="C269" s="6"/>
-      <c r="D269" s="7" t="s">
+      <c r="B269" s="22"/>
+      <c r="C269" s="18"/>
+      <c r="D269" s="3" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="270" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B270" s="5"/>
-      <c r="C270" s="6"/>
-      <c r="D270" s="7" t="s">
+      <c r="B270" s="22"/>
+      <c r="C270" s="18"/>
+      <c r="D270" s="3" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="271" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B271" s="8"/>
-      <c r="C271" s="9" t="s">
+      <c r="B271" s="23"/>
+      <c r="C271" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="D271" s="10"/>
+      <c r="D271" s="20"/>
     </row>
     <row r="272" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B272" s="2" t="s">
+      <c r="B272" s="21" t="s">
         <v>283</v>
       </c>
-      <c r="C272" s="3" t="s">
+      <c r="C272" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="D272" s="4" t="s">
+      <c r="D272" s="2" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="273" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B273" s="5"/>
-      <c r="C273" s="6"/>
-      <c r="D273" s="7" t="s">
+      <c r="B273" s="22"/>
+      <c r="C273" s="18"/>
+      <c r="D273" s="3" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="274" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B274" s="5"/>
-      <c r="C274" s="6"/>
-      <c r="D274" s="7" t="s">
+      <c r="B274" s="22"/>
+      <c r="C274" s="18"/>
+      <c r="D274" s="3" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="275" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B275" s="5"/>
-      <c r="C275" s="6"/>
-      <c r="D275" s="7" t="s">
+      <c r="B275" s="22"/>
+      <c r="C275" s="18"/>
+      <c r="D275" s="3" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="276" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B276" s="5"/>
-      <c r="C276" s="6"/>
-      <c r="D276" s="7" t="s">
+      <c r="B276" s="22"/>
+      <c r="C276" s="18"/>
+      <c r="D276" s="3" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="277" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B277" s="5"/>
-      <c r="C277" s="6"/>
-      <c r="D277" s="7" t="s">
+      <c r="B277" s="22"/>
+      <c r="C277" s="18"/>
+      <c r="D277" s="3" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="278" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B278" s="5"/>
-      <c r="C278" s="6"/>
-      <c r="D278" s="7" t="s">
+      <c r="B278" s="22"/>
+      <c r="C278" s="18"/>
+      <c r="D278" s="3" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="279" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B279" s="5"/>
-      <c r="C279" s="18" t="s">
+      <c r="B279" s="22"/>
+      <c r="C279" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D279" s="7" t="s">
+      <c r="D279" s="3" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="280" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B280" s="5"/>
-      <c r="C280" s="6" t="s">
+      <c r="B280" s="22"/>
+      <c r="C280" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D280" s="7" t="s">
+      <c r="D280" s="3" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="281" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B281" s="5"/>
-      <c r="C281" s="6"/>
-      <c r="D281" s="7" t="s">
+      <c r="B281" s="22"/>
+      <c r="C281" s="18"/>
+      <c r="D281" s="3" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="282" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B282" s="5"/>
-      <c r="C282" s="6"/>
-      <c r="D282" s="7" t="s">
+      <c r="B282" s="22"/>
+      <c r="C282" s="18"/>
+      <c r="D282" s="3" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="283" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B283" s="5"/>
-      <c r="C283" s="6"/>
-      <c r="D283" s="7" t="s">
+      <c r="B283" s="22"/>
+      <c r="C283" s="18"/>
+      <c r="D283" s="3" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="284" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B284" s="5"/>
-      <c r="C284" s="6"/>
-      <c r="D284" s="7" t="s">
+      <c r="B284" s="22"/>
+      <c r="C284" s="18"/>
+      <c r="D284" s="3" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="285" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B285" s="5"/>
-      <c r="C285" s="6" t="s">
+      <c r="B285" s="22"/>
+      <c r="C285" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="D285" s="7" t="s">
+      <c r="D285" s="3" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="286" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B286" s="5"/>
-      <c r="C286" s="6"/>
-      <c r="D286" s="7" t="s">
+      <c r="B286" s="22"/>
+      <c r="C286" s="18"/>
+      <c r="D286" s="3" t="s">
         <v>307</v>
       </c>
     </row>
     <row r="287" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B287" s="5"/>
-      <c r="C287" s="18" t="s">
+      <c r="B287" s="22"/>
+      <c r="C287" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D287" s="7" t="s">
+      <c r="D287" s="3" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="288" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B288" s="5"/>
-      <c r="C288" s="18" t="s">
+      <c r="B288" s="22"/>
+      <c r="C288" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D288" s="7" t="s">
+      <c r="D288" s="3" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="289" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B289" s="5"/>
-      <c r="C289" s="18" t="s">
+      <c r="B289" s="22"/>
+      <c r="C289" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="D289" s="7" t="s">
+      <c r="D289" s="3" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="290" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B290" s="5"/>
-      <c r="C290" s="6" t="s">
+      <c r="B290" s="22"/>
+      <c r="C290" s="18" t="s">
         <v>310</v>
       </c>
-      <c r="D290" s="7" t="s">
+      <c r="D290" s="3" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="291" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B291" s="5"/>
-      <c r="C291" s="6"/>
-      <c r="D291" s="7" t="s">
+      <c r="B291" s="22"/>
+      <c r="C291" s="18"/>
+      <c r="D291" s="3" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="292" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B292" s="5"/>
-      <c r="C292" s="6" t="s">
+      <c r="B292" s="22"/>
+      <c r="C292" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="D292" s="7" t="s">
+      <c r="D292" s="3" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="293" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B293" s="5"/>
-      <c r="C293" s="6"/>
-      <c r="D293" s="7" t="s">
+      <c r="B293" s="22"/>
+      <c r="C293" s="18"/>
+      <c r="D293" s="3" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="294" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B294" s="8"/>
-      <c r="C294" s="9" t="s">
+      <c r="B294" s="23"/>
+      <c r="C294" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="D294" s="10"/>
+      <c r="D294" s="20"/>
     </row>
     <row r="295" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B295" s="29" t="s">
+      <c r="B295" s="24" t="s">
         <v>315</v>
       </c>
-      <c r="C295" s="30"/>
-      <c r="D295" s="31"/>
+      <c r="C295" s="25"/>
+      <c r="D295" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="C285:C286"/>
-    <mergeCell ref="C290:C291"/>
-    <mergeCell ref="C292:C293"/>
-    <mergeCell ref="C294:D294"/>
+    <mergeCell ref="B2:B46"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="B48:B102"/>
+    <mergeCell ref="C102:D102"/>
+    <mergeCell ref="B103:B162"/>
+    <mergeCell ref="C2:C9"/>
+    <mergeCell ref="C10:C19"/>
+    <mergeCell ref="C20:C27"/>
+    <mergeCell ref="C28:C33"/>
+    <mergeCell ref="C34:C40"/>
+    <mergeCell ref="C41:C45"/>
+    <mergeCell ref="B163:B221"/>
+    <mergeCell ref="C222:C224"/>
+    <mergeCell ref="C230:C231"/>
+    <mergeCell ref="C163:C167"/>
+    <mergeCell ref="C168:C173"/>
+    <mergeCell ref="C174:C182"/>
+    <mergeCell ref="C183:C189"/>
+    <mergeCell ref="C190:C198"/>
+    <mergeCell ref="C199:C204"/>
+    <mergeCell ref="C205:C211"/>
     <mergeCell ref="B272:B294"/>
     <mergeCell ref="B295:D295"/>
     <mergeCell ref="C266:C270"/>
@@ -4422,29 +4438,13 @@
     <mergeCell ref="C242:C247"/>
     <mergeCell ref="C249:C250"/>
     <mergeCell ref="C252:C253"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="C285:C286"/>
+    <mergeCell ref="C290:C291"/>
+    <mergeCell ref="C292:C293"/>
+    <mergeCell ref="C294:D294"/>
     <mergeCell ref="C212:C217"/>
     <mergeCell ref="C218:C221"/>
-    <mergeCell ref="B163:B221"/>
-    <mergeCell ref="C222:C224"/>
-    <mergeCell ref="C230:C231"/>
-    <mergeCell ref="C163:C167"/>
-    <mergeCell ref="C168:C173"/>
-    <mergeCell ref="C174:C182"/>
-    <mergeCell ref="C183:C189"/>
-    <mergeCell ref="C190:C198"/>
-    <mergeCell ref="C199:C204"/>
-    <mergeCell ref="C205:C211"/>
-    <mergeCell ref="B2:B46"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="B48:B102"/>
-    <mergeCell ref="C102:D102"/>
-    <mergeCell ref="B103:B162"/>
-    <mergeCell ref="C2:C9"/>
-    <mergeCell ref="C10:C19"/>
-    <mergeCell ref="C20:C27"/>
-    <mergeCell ref="C28:C33"/>
-    <mergeCell ref="C34:C40"/>
-    <mergeCell ref="C41:C45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>